<commit_message>
-SmartFusion device roughly organized into separate blocks (symbols) -Pinout checked against BSDL file and datasheet -Pin names reflect names in BSDL file (i.e. I/O pins are named IO_<FBGA pin name>)
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
+++ b/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="438">
   <si>
     <t>Pin</t>
   </si>
@@ -1379,6 +1379,9 @@
   </si>
   <si>
     <t>A2F500 function (256-pin FPGA)</t>
+  </si>
+  <si>
+    <t>A2F500 function (256-pin FBGA)</t>
   </si>
 </sst>
 </file>
@@ -1743,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2284,7 +2287,7 @@
   <dimension ref="A1:B65"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:XFD230"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2823,8 +2826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3363,8 +3366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3379,7 +3382,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3896,5 +3899,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-All EAGLE SmartFusion device pin names follow the datasheet nomenclature (double-checked) -Main block organization follows SmartFusion EVAL/DEV board schematic
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
+++ b/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pins A1-D16 (1-64)" sheetId="2" r:id="rId1"/>
@@ -1746,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2286,8 +2286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2826,8 +2826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3366,8 +3366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updated pinout descriptions (mainly) for grounds.
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
+++ b/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="464">
   <si>
     <t>Pin</t>
   </si>
@@ -1381,14 +1381,92 @@
     <t>A2F500 function (256-pin FPGA)</t>
   </si>
   <si>
-    <t>A2F500 function (256-pin FBGA)</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Main function</t>
+  </si>
+  <si>
+    <t>Alternate function</t>
+  </si>
+  <si>
+    <t>Net name</t>
+  </si>
+  <si>
+    <t>Connected to</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Digital ground to the FPGA fabric, microcontroller subsystem and GPIOs</t>
+  </si>
+  <si>
+    <t>Quiet analog ground to the 1.5 V circuitry of the first analog-to-digital converter (ADC)</t>
+  </si>
+  <si>
+    <t>Quiet analog ground to the 1.5 V circuitry of the second ADC</t>
+  </si>
+  <si>
+    <t>Quiet analog ground to the 3.3 V circuitry of the second ADC</t>
+  </si>
+  <si>
+    <t>Quiet analog ground to the 3.3 V circuitry of the first ADC</t>
+  </si>
+  <si>
+    <t>Quiet analog ground to the analog front-end</t>
+  </si>
+  <si>
+    <t>Quiet analog ground to the analog I/O of SmartFusion devices</t>
+  </si>
+  <si>
+    <t>Digital ground to the embedded nonvolatile memory (eNVM)</t>
+  </si>
+  <si>
+    <t>Analog ground to the low power 32 KHz crystal oscillator circuitry</t>
+  </si>
+  <si>
+    <t>Analog ground to the main crystal oscillator circuitry</t>
+  </si>
+  <si>
+    <t>Quiet digital ground supply voltage to input buffers of I/O banks (see datasheet for details)</t>
+  </si>
+  <si>
+    <t>Analog ground to the integrated RC oscillator circuit</t>
+  </si>
+  <si>
+    <t>Analog ground to the first sigma-delta DAC</t>
+  </si>
+  <si>
+    <t>Common analog ground to the second and third sigma-delta DACs</t>
+  </si>
+  <si>
+    <t>Analog temperature monitor common ground for signal conditioning blocks SCB 0 and SB 1 (see datasheet for details)</t>
+  </si>
+  <si>
+    <t>Analog temperature monitor common ground for signal conditioning block SCB 2 and SCB 3 (see datasheet for details)</t>
+  </si>
+  <si>
+    <t>Analog ground reference used by the ADC (this pad should be connected to a quiet analog ground)</t>
+  </si>
+  <si>
+    <t>Digital supply to the FPGA fabric and MSS, nominally 1.5 V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1425,9 +1503,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1440,6 +1517,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1534,6 +1616,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1568,6 +1651,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1743,538 +1827,661 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="83.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H6" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+      <c r="C10" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H10" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+      <c r="C13" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="3" t="s">
+      <c r="C17" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H17" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+      <c r="C19" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H19" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="3" t="s">
+      <c r="C32" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H32" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="3" t="s">
+      <c r="C33" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H33" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="3" t="s">
+      <c r="C35" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="3" t="s">
+      <c r="C37" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="3" t="s">
+      <c r="C40" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H40" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="3" t="s">
+      <c r="C43" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="3" t="s">
+      <c r="C46" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H46" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="3" t="s">
+      <c r="C50" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="3" t="s">
+      <c r="C52" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H52" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="3" t="s">
+      <c r="C53" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H53" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="3" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="3" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="3" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="3" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="3" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="3" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="3" t="s">
+      <c r="C61" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H61" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="3" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>113</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -2283,538 +2490,742 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+      <c r="C7" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+      <c r="C9" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H9" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+      <c r="C10" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+      <c r="C11" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+      <c r="C12" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+      <c r="C19" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H19" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="3" t="s">
+      <c r="C24" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H24" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="3" t="s">
+      <c r="C25" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H25" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="3" t="s">
+      <c r="C26" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H26" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="3" t="s">
+      <c r="C27" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H27" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="3" t="s">
+      <c r="C28" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H28" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="3" t="s">
+      <c r="C30" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H30" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="3" t="s">
+      <c r="C32" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H32" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="3" t="s">
+      <c r="C33" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="3" t="s">
+      <c r="C39" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H39" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="3" t="s">
+      <c r="C40" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H40" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="3" t="s">
+      <c r="C41" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H41" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="3" t="s">
+      <c r="C42" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H42" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="3" t="s">
+      <c r="C43" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H43" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="3" t="s">
+      <c r="C44" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="3" t="s">
+      <c r="C45" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="3" t="s">
+      <c r="C49" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H49" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="3" t="s">
+      <c r="C50" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H50" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="3" t="s">
+      <c r="C52" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="3" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="3" t="s">
+      <c r="C55" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="3" t="s">
+      <c r="C56" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H56" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="3" t="s">
+      <c r="C57" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H57" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="3" t="s">
+      <c r="C58" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H58" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="3" t="s">
+      <c r="C59" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H59" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="3" t="s">
+      <c r="C60" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H60" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="3" t="s">
+      <c r="C61" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="3" t="s">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H65" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -2823,537 +3234,732 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="83.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+      <c r="C5" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H5" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+      <c r="C7" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H8" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+      <c r="C9" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H9" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+      <c r="C10" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H10" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+      <c r="C11" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+      <c r="C12" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+      <c r="C16" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="3" t="s">
+      <c r="C20" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="3" t="s">
+      <c r="C22" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="3" t="s">
+      <c r="C23" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="3" t="s">
+      <c r="C24" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H24" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="3" t="s">
+      <c r="C25" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H25" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="3" t="s">
+      <c r="C26" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H26" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="3" t="s">
+      <c r="C27" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H27" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="3" t="s">
+      <c r="C28" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H28" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="3" t="s">
+      <c r="C30" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H30" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="3" t="s">
+      <c r="C34" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H34" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="3" t="s">
+      <c r="C39" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H39" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="3" t="s">
+      <c r="C40" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H40" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="3" t="s">
+      <c r="C41" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H41" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="3" t="s">
+      <c r="C42" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H42" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="3" t="s">
+      <c r="C43" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H43" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="3" t="s">
+      <c r="C49" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H49" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="3" t="s">
+      <c r="C53" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H53" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="3" t="s">
+      <c r="C55" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H55" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="3" t="s">
+      <c r="C56" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H56" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="3" t="s">
+      <c r="C57" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H57" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="3" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="3" t="s">
+      <c r="C59" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H59" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="3" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="3" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="3" t="s">
+      <c r="C63" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="3" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>312</v>
       </c>
     </row>
@@ -3363,537 +3969,688 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+      <c r="C5" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H8" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+      <c r="C9" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+      <c r="C12" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H12" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
+      <c r="C14" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H14" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
+      <c r="C15" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+      <c r="C16" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H16" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="3" t="s">
+      <c r="C18" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H18" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+      <c r="C19" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="3" t="s">
+      <c r="C20" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="3" t="s">
+      <c r="C21" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H21" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="3" t="s">
+      <c r="C22" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H22" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="3" t="s">
+      <c r="C25" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="3" t="s">
+      <c r="C28" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H28" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="3" t="s">
+      <c r="C29" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="3" t="s">
+      <c r="C30" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H30" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="3" t="s">
+      <c r="C31" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="3" t="s">
+      <c r="C40" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="3" t="s">
+      <c r="C41" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="3" t="s">
+      <c r="C53" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H53" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="3" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="3" t="s">
+      <c r="C56" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H56" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="3" t="s">
+      <c r="C57" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H57" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="3" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="3" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="3" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="3" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="3" t="s">
+      <c r="C62" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H62" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="3" t="s">
+      <c r="C63" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H63" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="3" t="s">
+      <c r="C64" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>435</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a sketch of the 'North Bridge' mezzanine connector pinout.
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
+++ b/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Pins E1-H16 (65-128)" sheetId="4" r:id="rId2"/>
     <sheet name="Pins J1-M16 (129-92)" sheetId="5" r:id="rId3"/>
     <sheet name="Pins N1-T16 (193-256)" sheetId="6" r:id="rId4"/>
+    <sheet name="Calculations" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Pinout_1" localSheetId="0">'Pins A1-D16 (1-64)'!$A$1:$C$65</definedName>
@@ -18,7 +19,7 @@
     <definedName name="Pinout_1" localSheetId="2">'Pins J1-M16 (129-92)'!$A$1:$C$65</definedName>
     <definedName name="Pinout_1" localSheetId="3">'Pins N1-T16 (193-256)'!$A$1:$C$66</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="492">
   <si>
     <t>Pin</t>
   </si>
@@ -1405,9 +1406,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Digital ground to the FPGA fabric, microcontroller subsystem and GPIOs</t>
   </si>
   <si>
@@ -1460,13 +1458,100 @@
   </si>
   <si>
     <t>Digital supply to the FPGA fabric and MSS, nominally 1.5 V</t>
+  </si>
+  <si>
+    <t>Clean analog 1.5 V supply to the analog circuitry</t>
+  </si>
+  <si>
+    <t>Analog 1.5 V supply to the first ADC</t>
+  </si>
+  <si>
+    <t>Analog 1.5 V supply to the second ADC</t>
+  </si>
+  <si>
+    <t>Clean 3.3 V analog supply to the analog circuitry (see documentation for more details)</t>
+  </si>
+  <si>
+    <t>Analog 3.3 V supply to the first ADC</t>
+  </si>
+  <si>
+    <t>Analog 3.3 V supply to the second ADC</t>
+  </si>
+  <si>
+    <t>Analog clean 3.3 V supply to the charge pump</t>
+  </si>
+  <si>
+    <t>–3.3 V output from the voltage converter (a 2.2 μF capacitor must be connected from this pin to GND)</t>
+  </si>
+  <si>
+    <t>Analog 3.3 V supply to the first sigma-delta DAC</t>
+  </si>
+  <si>
+    <t>Common analog 3.3 V supply to the second and third sigma-delta DACs</t>
+  </si>
+  <si>
+    <t>Digital 1.5 V power supply to the embedded nonvolatile memory blocks</t>
+  </si>
+  <si>
+    <t>Digital supply to the FPGA fabric I/O bank 0 (north FPGA I/O bank) for the output buffers and I/O logic</t>
+  </si>
+  <si>
+    <t>Digital supply to the FPGA fabric I/O bank 1 (east FPGA I/O bank) for the output buffers and I/O logic</t>
+  </si>
+  <si>
+    <t>Analog supply to the low power 32 KHz crystal oscillator</t>
+  </si>
+  <si>
+    <t>Analog supply to the main crystal oscillator circuit</t>
+  </si>
+  <si>
+    <t>Digital supply to the FPGA fabric I/O bank 2 (east MSS I/O bank) for the output buffers and I/O logic</t>
+  </si>
+  <si>
+    <t>Digital supply to the FPGA fabric I/O bank 4 (west MSS I/O bank) for the output buffers and I/O logic</t>
+  </si>
+  <si>
+    <t>Analog 1.5 V supply to the PLL</t>
+  </si>
+  <si>
+    <t>Analog supply to the integrated RC oscillator circuit</t>
+  </si>
+  <si>
+    <t>Analog ground for the PLL</t>
+  </si>
+  <si>
+    <t>Digital supply to the FPGA fabric I/O bank 5 (west FPGA I/O bank) for the output buffers and I/O logic</t>
+  </si>
+  <si>
+    <t>External battery connection to the low power 32 KHz crystal oscillator (along with VCCLPXTAL), RTC, and battery switchover circuit</t>
+  </si>
+  <si>
+    <t>Digital supply to the JTAG controller</t>
+  </si>
+  <si>
+    <t>Digital programming circuitry supply*</t>
+  </si>
+  <si>
+    <t>Analog reference voltage for second ADC*</t>
+  </si>
+  <si>
+    <t>Analog reference voltage for first ADC*</t>
+  </si>
+  <si>
+    <t>Internal 2.56 V voltage reference output</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>D3V3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1482,13 +1567,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1500,10 +1609,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1511,11 +1622,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1830,8 +1992,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,7 +2006,7 @@
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="83.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="92.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1877,7 +2040,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1887,11 +2050,11 @@
         <v>444</v>
       </c>
       <c r="H2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1899,6 +2062,15 @@
       </c>
       <c r="C3" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="F3" t="s">
+        <v>491</v>
+      </c>
+      <c r="G3" t="s">
+        <v>490</v>
+      </c>
+      <c r="H3" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1918,7 +2090,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1928,7 +2100,7 @@
         <v>444</v>
       </c>
       <c r="H6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1948,15 +2120,21 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H9" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1966,7 +2144,7 @@
         <v>444</v>
       </c>
       <c r="H10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1986,7 +2164,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1996,7 +2174,7 @@
         <v>444</v>
       </c>
       <c r="H13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2016,15 +2194,21 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H16" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2034,7 +2218,7 @@
         <v>444</v>
       </c>
       <c r="H17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2046,7 +2230,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2056,7 +2240,7 @@
         <v>444</v>
       </c>
       <c r="H19" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2156,7 +2340,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -2166,7 +2350,7 @@
         <v>444</v>
       </c>
       <c r="H32" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2180,7 +2364,7 @@
         <v>444</v>
       </c>
       <c r="H33" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2192,7 +2376,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2200,6 +2384,9 @@
       </c>
       <c r="C35" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="H35" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2211,7 +2398,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -2219,6 +2406,9 @@
       </c>
       <c r="C37" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="H37" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2238,7 +2428,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -2248,7 +2438,7 @@
         <v>444</v>
       </c>
       <c r="H40" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2268,7 +2458,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -2276,6 +2466,9 @@
       </c>
       <c r="C43" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="H43" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2295,7 +2488,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -2305,7 +2498,7 @@
         <v>444</v>
       </c>
       <c r="H46" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2333,7 +2526,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -2342,17 +2535,26 @@
       <c r="C50" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H50" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="C51" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H51" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -2362,7 +2564,7 @@
         <v>444</v>
       </c>
       <c r="H52" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2376,7 +2578,7 @@
         <v>444</v>
       </c>
       <c r="H53" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2446,7 +2648,7 @@
         <v>444</v>
       </c>
       <c r="H61" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2473,8 +2675,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B65" s="2" t="s">
@@ -2483,9 +2685,23 @@
       <c r="C65" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H65" t="s">
+        <v>475</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="beginsWith" dxfId="5" priority="2" operator="beginsWith" text="S">
+      <formula>LEFT(C1,LEN("S"))="S"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="VCC">
+      <formula>LEFT(B1,LEN("VCC"))="VCC"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2493,8 +2709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2506,7 +2722,7 @@
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="92.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2582,11 +2798,11 @@
         <v>444</v>
       </c>
       <c r="H6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>123</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2596,11 +2812,11 @@
         <v>444</v>
       </c>
       <c r="H7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2609,9 +2825,12 @@
       <c r="C8" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H8" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2621,11 +2840,11 @@
         <v>444</v>
       </c>
       <c r="H9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2634,9 +2853,12 @@
       <c r="C10" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H10" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2646,11 +2868,11 @@
         <v>444</v>
       </c>
       <c r="H11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>128</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -2658,6 +2880,9 @@
       </c>
       <c r="C12" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="H12" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2669,11 +2894,17 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>113</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H14" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2709,7 +2940,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2719,7 +2950,7 @@
         <v>444</v>
       </c>
       <c r="H19" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2731,11 +2962,17 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>86</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H21" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2747,15 +2984,21 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="C23" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H23" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>147</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -2765,11 +3008,11 @@
         <v>444</v>
       </c>
       <c r="H24" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2779,11 +3022,11 @@
         <v>444</v>
       </c>
       <c r="H25" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>150</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -2793,11 +3036,11 @@
         <v>444</v>
       </c>
       <c r="H26" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>151</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2807,11 +3050,11 @@
         <v>444</v>
       </c>
       <c r="H27" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>152</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -2821,7 +3064,7 @@
         <v>444</v>
       </c>
       <c r="H28" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2843,7 +3086,7 @@
         <v>444</v>
       </c>
       <c r="H30" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2855,7 +3098,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="3" t="s">
         <v>158</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -2865,11 +3108,11 @@
         <v>444</v>
       </c>
       <c r="H32" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="3" t="s">
         <v>159</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -2877,6 +3120,9 @@
       </c>
       <c r="C33" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="H33" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2920,7 +3166,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>171</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -2930,11 +3176,11 @@
         <v>444</v>
       </c>
       <c r="H39" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>172</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -2944,11 +3190,11 @@
         <v>444</v>
       </c>
       <c r="H40" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>173</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -2958,11 +3204,11 @@
         <v>444</v>
       </c>
       <c r="H41" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>174</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -2972,11 +3218,11 @@
         <v>444</v>
       </c>
       <c r="H42" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>175</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -2986,11 +3232,11 @@
         <v>444</v>
       </c>
       <c r="H43" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>176</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -2998,6 +3244,9 @@
       </c>
       <c r="C44" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="H44" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3008,7 +3257,10 @@
         <v>178</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
+      </c>
+      <c r="H45" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3036,7 +3288,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="3" t="s">
         <v>185</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -3046,11 +3298,11 @@
         <v>444</v>
       </c>
       <c r="H49" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="3" t="s">
         <v>187</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -3060,7 +3312,7 @@
         <v>444</v>
       </c>
       <c r="H50" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3072,7 +3324,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="3" t="s">
         <v>190</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -3080,6 +3332,9 @@
       </c>
       <c r="C52" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="H52" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -3099,7 +3354,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="3" t="s">
         <v>195</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -3108,9 +3363,12 @@
       <c r="C55" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H55" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="3" t="s">
         <v>196</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -3120,11 +3378,11 @@
         <v>444</v>
       </c>
       <c r="H56" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="3" t="s">
         <v>197</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -3134,11 +3392,11 @@
         <v>444</v>
       </c>
       <c r="H57" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="3" t="s">
         <v>198</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -3148,11 +3406,11 @@
         <v>444</v>
       </c>
       <c r="H58" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="3" t="s">
         <v>199</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -3162,11 +3420,11 @@
         <v>444</v>
       </c>
       <c r="H59" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="3" t="s">
         <v>200</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -3176,7 +3434,7 @@
         <v>444</v>
       </c>
       <c r="H60" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -3189,6 +3447,9 @@
       <c r="C61" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H61" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
@@ -3215,7 +3476,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="3" t="s">
         <v>209</v>
       </c>
       <c r="B65" s="2" t="s">
@@ -3225,10 +3486,18 @@
         <v>444</v>
       </c>
       <c r="H65" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="beginsWith" priority="2" operator="beginsWith" text="VCC">
+      <formula>LEFT(B1,LEN("VCC"))="VCC"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="1" operator="beginsWith" text="VCC">
+      <formula>LEFT(B1,LEN("VCC"))="VCC"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3237,8 +3506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3250,7 +3519,7 @@
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="83.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="107.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3308,7 +3577,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>216</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -3318,7 +3587,7 @@
         <v>444</v>
       </c>
       <c r="H5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3332,11 +3601,11 @@
         <v>444</v>
       </c>
       <c r="H6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>219</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -3346,11 +3615,11 @@
         <v>444</v>
       </c>
       <c r="H7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>220</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -3360,11 +3629,11 @@
         <v>444</v>
       </c>
       <c r="H8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>221</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -3374,11 +3643,11 @@
         <v>444</v>
       </c>
       <c r="H9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>222</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -3388,11 +3657,11 @@
         <v>444</v>
       </c>
       <c r="H10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>223</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -3402,11 +3671,11 @@
         <v>444</v>
       </c>
       <c r="H11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>224</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -3414,6 +3683,9 @@
       </c>
       <c r="C12" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="H12" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3441,7 +3713,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>232</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -3449,6 +3721,9 @@
       </c>
       <c r="C16" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="H16" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -3476,7 +3751,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>239</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -3484,6 +3759,9 @@
       </c>
       <c r="C20" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="H20" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -3495,7 +3773,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="4" t="s">
         <v>243</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -3504,9 +3782,12 @@
       <c r="C22" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H22" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>245</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -3515,9 +3796,12 @@
       <c r="C23" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H23" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>246</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -3527,11 +3811,11 @@
         <v>444</v>
       </c>
       <c r="H24" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>247</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -3541,11 +3825,11 @@
         <v>444</v>
       </c>
       <c r="H25" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -3555,11 +3839,11 @@
         <v>444</v>
       </c>
       <c r="H26" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>249</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -3569,11 +3853,11 @@
         <v>444</v>
       </c>
       <c r="H27" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>250</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -3583,7 +3867,7 @@
         <v>444</v>
       </c>
       <c r="H28" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3595,7 +3879,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>253</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -3605,7 +3889,7 @@
         <v>444</v>
       </c>
       <c r="H30" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3633,7 +3917,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="3" t="s">
         <v>260</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -3643,7 +3927,7 @@
         <v>444</v>
       </c>
       <c r="H34" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3679,7 +3963,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>269</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -3689,11 +3973,11 @@
         <v>444</v>
       </c>
       <c r="H39" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>270</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -3703,11 +3987,11 @@
         <v>444</v>
       </c>
       <c r="H40" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>271</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -3717,11 +4001,11 @@
         <v>444</v>
       </c>
       <c r="H41" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>272</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -3731,11 +4015,11 @@
         <v>444</v>
       </c>
       <c r="H42" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>273</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -3745,15 +4029,21 @@
         <v>444</v>
       </c>
       <c r="H43" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>274</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>225</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="H44" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3789,7 +4079,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="3" t="s">
         <v>283</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -3799,7 +4089,7 @@
         <v>444</v>
       </c>
       <c r="H49" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3827,7 +4117,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="3" t="s">
         <v>290</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -3837,7 +4127,7 @@
         <v>444</v>
       </c>
       <c r="H53" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3859,7 +4149,7 @@
         <v>444</v>
       </c>
       <c r="H55" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3873,7 +4163,7 @@
         <v>444</v>
       </c>
       <c r="H56" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -3887,7 +4177,7 @@
         <v>444</v>
       </c>
       <c r="H57" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3909,7 +4199,7 @@
         <v>444</v>
       </c>
       <c r="H59" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -3937,7 +4227,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="3" t="s">
         <v>308</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -3945,6 +4235,9 @@
       </c>
       <c r="C63" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="H63" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -3972,9 +4265,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H63" sqref="H63"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3986,7 +4279,7 @@
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" customWidth="1"/>
-    <col min="8" max="8" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="107.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4028,7 +4321,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>315</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4036,6 +4329,9 @@
       </c>
       <c r="C3" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="H3" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4048,6 +4344,9 @@
       <c r="C4" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H4" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -4059,6 +4358,9 @@
       <c r="C5" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H5" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -4087,7 +4389,7 @@
         <v>444</v>
       </c>
       <c r="H8" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -4100,6 +4402,9 @@
       <c r="C9" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H9" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -4128,7 +4433,7 @@
         <v>444</v>
       </c>
       <c r="H12" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4138,6 +4443,9 @@
       <c r="B13" s="2" t="s">
         <v>335</v>
       </c>
+      <c r="H13" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -4150,7 +4458,7 @@
         <v>444</v>
       </c>
       <c r="H14" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4163,9 +4471,12 @@
       <c r="C15" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H15" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>340</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -4175,7 +4486,7 @@
         <v>444</v>
       </c>
       <c r="H16" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -4197,7 +4508,7 @@
         <v>444</v>
       </c>
       <c r="H18" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -4210,6 +4521,9 @@
       <c r="C19" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H19" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -4221,6 +4535,9 @@
       <c r="C20" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H20" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -4233,7 +4550,7 @@
         <v>444</v>
       </c>
       <c r="H21" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -4247,7 +4564,7 @@
         <v>444</v>
       </c>
       <c r="H22" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -4276,6 +4593,9 @@
       <c r="C25" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H25" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -4304,7 +4624,7 @@
         <v>444</v>
       </c>
       <c r="H28" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -4317,6 +4637,9 @@
       <c r="C29" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H29" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
@@ -4329,7 +4652,7 @@
         <v>444</v>
       </c>
       <c r="H30" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -4342,6 +4665,9 @@
       <c r="C31" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="H31" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -4351,7 +4677,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>371</v>
       </c>
@@ -4359,7 +4685,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>373</v>
       </c>
@@ -4367,7 +4693,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>375</v>
       </c>
@@ -4375,7 +4701,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>377</v>
       </c>
@@ -4383,7 +4709,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>379</v>
       </c>
@@ -4391,7 +4717,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>381</v>
       </c>
@@ -4399,7 +4725,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>383</v>
       </c>
@@ -4407,7 +4733,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>385</v>
       </c>
@@ -4417,8 +4743,11 @@
       <c r="C40" s="2" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>387</v>
       </c>
@@ -4428,8 +4757,11 @@
       <c r="C41" s="2" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>389</v>
       </c>
@@ -4437,7 +4769,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>391</v>
       </c>
@@ -4445,7 +4777,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>393</v>
       </c>
@@ -4453,7 +4785,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>395</v>
       </c>
@@ -4461,7 +4793,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>397</v>
       </c>
@@ -4469,7 +4801,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>399</v>
       </c>
@@ -4477,7 +4809,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>401</v>
       </c>
@@ -4492,6 +4824,9 @@
       <c r="B49" s="2" t="s">
         <v>404</v>
       </c>
+      <c r="H49" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
@@ -4528,7 +4863,7 @@
         <v>444</v>
       </c>
       <c r="H53" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -4546,6 +4881,9 @@
       <c r="B55" s="2" t="s">
         <v>416</v>
       </c>
+      <c r="H55" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
@@ -4558,7 +4896,7 @@
         <v>444</v>
       </c>
       <c r="H56" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -4572,7 +4910,7 @@
         <v>444</v>
       </c>
       <c r="H57" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -4582,6 +4920,9 @@
       <c r="B58" s="2" t="s">
         <v>421</v>
       </c>
+      <c r="H58" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
@@ -4618,7 +4959,7 @@
         <v>444</v>
       </c>
       <c r="H62" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -4632,7 +4973,7 @@
         <v>444</v>
       </c>
       <c r="H63" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -4644,6 +4985,9 @@
       </c>
       <c r="C64" s="2" t="s">
         <v>444</v>
+      </c>
+      <c r="H64" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -4658,4 +5002,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Worked on pinout assignment and converted project into Eagle v6 format.
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
+++ b/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Pins J1-M16 (129-92)" sheetId="5" r:id="rId3"/>
     <sheet name="Pins N1-T16 (193-256)" sheetId="6" r:id="rId4"/>
     <sheet name="Calculations" sheetId="7" r:id="rId5"/>
+    <sheet name="Legend" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Pinout_1" localSheetId="0">'Pins A1-D16 (1-64)'!$A$1:$C$65</definedName>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="502">
   <si>
     <t>Pin</t>
   </si>
@@ -1545,13 +1546,43 @@
   </si>
   <si>
     <t>D3V3</t>
+  </si>
+  <si>
+    <t>Pin color</t>
+  </si>
+  <si>
+    <t>Pins checked against datasheet</t>
+  </si>
+  <si>
+    <t>Routed on the board</t>
+  </si>
+  <si>
+    <t>Connected on the schematic</t>
+  </si>
+  <si>
+    <t>Tested in Libero Design</t>
+  </si>
+  <si>
+    <t>CLKA Hardwired I/O</t>
+  </si>
+  <si>
+    <t>Main oscillator IN</t>
+  </si>
+  <si>
+    <t>Main oscillator OUT</t>
+  </si>
+  <si>
+    <t>Low-power oscillator IN</t>
+  </si>
+  <si>
+    <t>Low-power oscillator OUT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1581,8 +1612,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1599,6 +1645,17 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1609,12 +1666,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1628,27 +1687,24 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="60% - Accent1" xfId="4" builtinId="32"/>
+    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -1667,6 +1723,13 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1993,13 +2056,13 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.5703125" customWidth="1"/>
@@ -2691,13 +2754,8 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="beginsWith" dxfId="5" priority="2" operator="beginsWith" text="S">
+    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="S">
       <formula>LEFT(C1,LEN("S"))="S"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="VCC">
-      <formula>LEFT(B1,LEN("VCC"))="VCC"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2709,8 +2767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2772,11 +2830,14 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>119</v>
+      </c>
+      <c r="H4" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -3491,10 +3552,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="beginsWith" priority="2" operator="beginsWith" text="VCC">
+    <cfRule type="beginsWith" dxfId="0" priority="1" operator="beginsWith" text="VCC">
       <formula>LEFT(B1,LEN("VCC"))="VCC"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="1" operator="beginsWith" text="VCC">
+    <cfRule type="beginsWith" priority="2" operator="beginsWith" text="VCC">
       <formula>LEFT(B1,LEN("VCC"))="VCC"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3507,7 +3568,7 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3765,7 +3826,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="4" t="s">
         <v>241</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -4266,8 +4327,8 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45:A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4786,35 +4847,47 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="4" t="s">
         <v>395</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>396</v>
       </c>
+      <c r="H45" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="4" t="s">
         <v>397</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>398</v>
       </c>
+      <c r="H46" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="4" t="s">
         <v>399</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>400</v>
       </c>
+      <c r="H47" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="4" t="s">
         <v>401</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>402</v>
+      </c>
+      <c r="H48" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -5014,4 +5087,61 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>493</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>496</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>495</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>494</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Clock signals checked in datasheet and Libero, and added to schematic with the exception of the ADC clocks.
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
+++ b/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pins A1-D16 (1-64)" sheetId="2" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="534">
   <si>
     <t>Pin</t>
   </si>
@@ -318,9 +318,6 @@
     <t>C15</t>
   </si>
   <si>
-    <t>GCA2/IO28PDB1V0</t>
-  </si>
-  <si>
     <t>C16</t>
   </si>
   <si>
@@ -429,9 +426,6 @@
     <t>E3</t>
   </si>
   <si>
-    <t>GFA2/IO85PDB5V0</t>
-  </si>
-  <si>
     <t>E4</t>
   </si>
   <si>
@@ -498,9 +492,6 @@
     <t>F3</t>
   </si>
   <si>
-    <t>GFB2/IO85NDB5V0</t>
-  </si>
-  <si>
     <t>F4</t>
   </si>
   <si>
@@ -1563,9 +1554,6 @@
     <t>Tested in Libero Design</t>
   </si>
   <si>
-    <t>CLKA Hardwired I/O</t>
-  </si>
-  <si>
     <t>Main oscillator IN</t>
   </si>
   <si>
@@ -1576,6 +1564,174 @@
   </si>
   <si>
     <t>Low-power oscillator OUT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GFA2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/IO85PDB5V0</t>
+    </r>
+  </si>
+  <si>
+    <t>FOX924 20 MHz TCXO</t>
+  </si>
+  <si>
+    <t>GF CCC (MSS_CCC) CLKA hardwired I/O</t>
+  </si>
+  <si>
+    <t>GF CCC (MSS_CCC) CLKB hardwired I/O</t>
+  </si>
+  <si>
+    <t>MAIN_CLK_IN</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>EXT_CLK_IN</t>
+  </si>
+  <si>
+    <t>SMA connector</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GFB2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/IO85NDB5V0</t>
+    </r>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t># of pins</t>
+  </si>
+  <si>
+    <t>Clock</t>
+  </si>
+  <si>
+    <t>REF_CLK_OUT</t>
+  </si>
+  <si>
+    <t>EXT_CLK_OUT</t>
+  </si>
+  <si>
+    <t>USB_CLK_IN</t>
+  </si>
+  <si>
+    <t>Candidate pins</t>
+  </si>
+  <si>
+    <t>GCxx</t>
+  </si>
+  <si>
+    <t>Any with OBUF</t>
+  </si>
+  <si>
+    <t>Unassigned pins</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GCA2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/IO28PDB1V0</t>
+    </r>
+  </si>
+  <si>
+    <t>GC CCC (Middle CCC) CLKA single-ended hardwired I/O</t>
+  </si>
+  <si>
+    <t>Single ended clock for the FTDI USB block</t>
+  </si>
+  <si>
+    <t>FTDI FT232H USB</t>
+  </si>
+  <si>
+    <t>Can be moved to any GCxx dedicated clock input pin</t>
+  </si>
+  <si>
+    <t>Initial pin assignment</t>
+  </si>
+  <si>
+    <t>C15 (GCA2)</t>
+  </si>
+  <si>
+    <t>Can be moved to any GCxx pin</t>
+  </si>
+  <si>
+    <t>Can be relocated to any output pin and merged with EXT_CLK_OUT</t>
+  </si>
+  <si>
+    <t>Can be relocated to any output pin and merged with REF_CLK_OUT</t>
+  </si>
+  <si>
+    <t>USB_CLK</t>
+  </si>
+  <si>
+    <t>Mezzanine connector</t>
+  </si>
+  <si>
+    <t>FPGA user I/O</t>
+  </si>
+  <si>
+    <t>Can be relocated to any other I/O and merged with EXT_CLK_OUT</t>
+  </si>
+  <si>
+    <t>Can be relocated to any other I/O and merged with REF_CLK_OUT</t>
+  </si>
+  <si>
+    <t>20 MHz reference clock out</t>
+  </si>
+  <si>
+    <t>I/O</t>
   </si>
 </sst>
 </file>
@@ -1673,7 +1829,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1696,6 +1852,15 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="60% - Accent1" xfId="4" builtinId="32"/>
@@ -1704,28 +1869,7 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -2055,9 +2199,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2065,12 +2209,12 @@
     <col min="1" max="1" width="7.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="92.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2078,28 +2222,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2110,10 +2254,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H2" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2124,16 +2268,16 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="G3" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="H3" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2160,10 +2304,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H6" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2190,10 +2334,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H9" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2204,10 +2348,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H10" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2234,10 +2378,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H13" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2264,10 +2408,10 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H16" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2278,10 +2422,10 @@
         <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H17" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2300,10 +2444,10 @@
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H19" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2410,13 +2554,13 @@
         <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H32" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>55</v>
       </c>
@@ -2424,13 +2568,13 @@
         <v>56</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H33" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>57</v>
       </c>
@@ -2438,7 +2582,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>59</v>
       </c>
@@ -2446,13 +2590,13 @@
         <v>60</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H35" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>61</v>
       </c>
@@ -2460,7 +2604,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>63</v>
       </c>
@@ -2468,13 +2612,13 @@
         <v>4</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H37" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>64</v>
       </c>
@@ -2482,7 +2626,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
@@ -2490,7 +2634,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>68</v>
       </c>
@@ -2498,13 +2642,13 @@
         <v>2</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H40" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>69</v>
       </c>
@@ -2512,7 +2656,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>71</v>
       </c>
@@ -2520,7 +2664,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>73</v>
       </c>
@@ -2528,13 +2672,13 @@
         <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H43" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>74</v>
       </c>
@@ -2542,7 +2686,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>76</v>
       </c>
@@ -2550,7 +2694,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>78</v>
       </c>
@@ -2558,13 +2702,13 @@
         <v>2</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H46" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>79</v>
       </c>
@@ -2572,189 +2716,207 @@
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>81</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>82</v>
+        <v>517</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="D48" t="s">
+        <v>519</v>
+      </c>
+      <c r="F48" t="s">
+        <v>512</v>
+      </c>
+      <c r="G48" t="s">
+        <v>520</v>
+      </c>
+      <c r="H48" t="s">
+        <v>518</v>
+      </c>
+      <c r="I48" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="C50" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H50" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="C51" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H51" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H52" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H53" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H61" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="C65" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H65" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="S">
+    <cfRule type="beginsWith" dxfId="1" priority="2" operator="beginsWith" text="S">
       <formula>LEFT(C1,LEN("S"))="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2767,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2778,8 +2940,8 @@
     <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="92.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.85546875" customWidth="1"/>
   </cols>
@@ -2789,765 +2951,924 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>115</v>
+      <c r="C2" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H2" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H3" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>118</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>119</v>
+        <v>498</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>499</v>
       </c>
       <c r="H4" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H5" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H7" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H8" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H9" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H10" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H11" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H12" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H13" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H14" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H15" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H16" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H17" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H18" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H19" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>141</v>
+      <c r="A20" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>142</v>
+        <v>506</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="H20" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H21" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H22" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H23" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H24" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H25" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H26" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H27" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H28" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H29" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H30" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H31" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H32" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H33" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C34" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H34" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="H33" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C35" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H35" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C36" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H36" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C37" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="D37" t="s">
+        <v>532</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="H37" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C38" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="D38" t="s">
+        <v>532</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="H38" t="s">
+        <v>529</v>
+      </c>
+      <c r="I38" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H39" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+      <c r="I39" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H40" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H41" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H42" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H43" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H44" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H45" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="H44" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B45" s="2" t="s">
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="H45" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B46" s="2" t="s">
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H49" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H50" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H51" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H52" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H53" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="H54" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H55" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H56" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H57" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H58" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H59" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H60" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H61" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H65" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -3560,6 +3881,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3567,8 +3889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3589,732 +3911,732 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H5" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H7" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H8" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H9" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H10" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H11" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H12" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H16" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H20" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H22" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H23" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H24" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H25" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H26" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H27" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H28" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H30" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H34" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H39" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H40" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H41" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H42" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H43" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H44" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H49" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H53" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H55" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H56" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H57" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H59" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H63" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -4328,7 +4650,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45:A48"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4349,726 +4671,726 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H4" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H8" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H9" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H12" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H13" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H14" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H15" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H16" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H18" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H19" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H20" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H21" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H22" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H25" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H28" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H29" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H30" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H31" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H40" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H41" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="H45" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="B46" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="H46" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="H45" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="B47" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="H47" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="H46" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="B48" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="H47" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>401</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>402</v>
-      </c>
       <c r="H48" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="H49" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H53" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H55" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H56" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H57" t="s">
         <v>444</v>
-      </c>
-      <c r="H57" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H58" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H62" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H63" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H64" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -5079,12 +5401,113 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="59.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="F5" t="s">
+        <v>524</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5105,12 +5528,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -5118,7 +5541,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
@@ -5126,7 +5549,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -5134,7 +5557,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Connected the external analog front-ends (MAX19706) in schematic.
-Auxiliary ADCs/DACs are not connected yet
-FPGA-MAX19706 connections are not final
</commit_message>
<xml_diff>
--- a/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
+++ b/hardware/MainBoard/Document/A2F500 FT256 Pinout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Pins A1-D16 (1-64)" sheetId="2" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="538">
   <si>
     <t>Pin</t>
   </si>
@@ -1648,9 +1648,6 @@
     <t>EXT_CLK_OUT</t>
   </si>
   <si>
-    <t>USB_CLK_IN</t>
-  </si>
-  <si>
     <t>Candidate pins</t>
   </si>
   <si>
@@ -1689,9 +1686,6 @@
     <t>GC CCC (Middle CCC) CLKA single-ended hardwired I/O</t>
   </si>
   <si>
-    <t>Single ended clock for the FTDI USB block</t>
-  </si>
-  <si>
     <t>FTDI FT232H USB</t>
   </si>
   <si>
@@ -1732,13 +1726,31 @@
   </si>
   <si>
     <t>I/O</t>
+  </si>
+  <si>
+    <t>Initial assignment (may be relocated)</t>
+  </si>
+  <si>
+    <t>Single ended clock for USB from the FTDI chip</t>
+  </si>
+  <si>
+    <t>Single ended clock to the analog front-ends</t>
+  </si>
+  <si>
+    <t>AFE_CLK</t>
+  </si>
+  <si>
+    <t>MAX19706</t>
+  </si>
+  <si>
+    <t>Can be moved to any FPGA I/O output pin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1783,6 +1795,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1813,7 +1833,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1821,15 +1841,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1852,18 +1888,22 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="60% - Accent1" xfId="4" builtinId="32"/>
+    <cellStyle name="Calculation" xfId="5" builtinId="22"/>
     <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
@@ -2199,9 +2239,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,7 +2249,7 @@
     <col min="1" max="1" width="7.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" customWidth="1"/>
@@ -2717,40 +2757,58 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="9" t="s">
         <v>81</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>503</v>
       </c>
       <c r="D48" t="s">
+        <v>533</v>
+      </c>
+      <c r="F48" t="s">
+        <v>525</v>
+      </c>
+      <c r="G48" t="s">
+        <v>518</v>
+      </c>
+      <c r="H48" t="s">
+        <v>517</v>
+      </c>
+      <c r="I48" t="s">
         <v>519</v>
       </c>
-      <c r="F48" t="s">
-        <v>512</v>
-      </c>
-      <c r="G48" t="s">
-        <v>520</v>
-      </c>
-      <c r="H48" t="s">
-        <v>518</v>
-      </c>
-      <c r="I48" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
         <v>82</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="D49" t="s">
+        <v>534</v>
+      </c>
+      <c r="F49" t="s">
+        <v>535</v>
+      </c>
+      <c r="G49" t="s">
+        <v>536</v>
+      </c>
+      <c r="H49" t="s">
+        <v>527</v>
+      </c>
+      <c r="I49" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>84</v>
       </c>
@@ -2764,7 +2822,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>86</v>
       </c>
@@ -2778,7 +2836,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>88</v>
       </c>
@@ -2792,7 +2850,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>89</v>
       </c>
@@ -2806,7 +2864,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>90</v>
       </c>
@@ -2814,7 +2872,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>92</v>
       </c>
@@ -2822,7 +2880,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>94</v>
       </c>
@@ -2830,7 +2888,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>96</v>
       </c>
@@ -2838,7 +2896,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>98</v>
       </c>
@@ -2846,7 +2904,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>100</v>
       </c>
@@ -2854,7 +2912,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>102</v>
       </c>
@@ -2862,7 +2920,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>104</v>
       </c>
@@ -2876,7 +2934,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>105</v>
       </c>
@@ -2884,7 +2942,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>107</v>
       </c>
@@ -2892,7 +2950,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>109</v>
       </c>
@@ -2929,8 +2987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2983,10 +3041,10 @@
         <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2997,10 +3055,10 @@
         <v>116</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H3" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -3031,10 +3089,10 @@
         <v>119</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H5" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3143,10 +3201,10 @@
         <v>128</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H13" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3171,10 +3229,10 @@
         <v>131</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H15" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3185,10 +3243,10 @@
         <v>133</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H16" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -3199,10 +3257,10 @@
         <v>135</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H17" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -3213,10 +3271,10 @@
         <v>137</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H18" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -3275,10 +3333,10 @@
         <v>142</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H22" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -3373,10 +3431,10 @@
         <v>151</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H29" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3401,10 +3459,10 @@
         <v>154</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H31" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3443,10 +3501,10 @@
         <v>159</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H34" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3457,10 +3515,10 @@
         <v>161</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H35" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3471,47 +3529,47 @@
         <v>163</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H36" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="9" t="s">
         <v>164</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D37" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>510</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="H37" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="9" t="s">
         <v>166</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>167</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D38" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>511</v>
@@ -3520,10 +3578,10 @@
         <v>505</v>
       </c>
       <c r="H38" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="I38" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3540,7 +3598,7 @@
         <v>442</v>
       </c>
       <c r="I39" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3687,10 +3745,10 @@
         <v>186</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H51" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -3715,10 +3773,10 @@
         <v>189</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H53" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3729,10 +3787,10 @@
         <v>191</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H54" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -5418,14 +5476,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>516</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="A1" s="11" t="s">
+        <v>515</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -5435,10 +5493,10 @@
         <v>508</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>439</v>
@@ -5448,7 +5506,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>509</v>
       </c>
       <c r="B3" s="2">
@@ -5458,17 +5516,17 @@
         <v>164</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>525</v>
+      <c r="F3" s="8" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -5476,31 +5534,31 @@
         <v>166</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>526</v>
+      <c r="F4" s="8" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="2">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="F5" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -5514,15 +5572,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -5557,9 +5615,17 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>532</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>491</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>